<commit_message>
new data on Amgen
</commit_message>
<xml_diff>
--- a/Dow 30/Amgen/Amgen DCF.xlsx
+++ b/Dow 30/Amgen/Amgen DCF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogdan\Desktop\shashwat\DCF\Dow 30\Amgen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\DCF\Dow 30\Amgen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B8D6EA-B211-4BC3-BC32-5DC69636E949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB575EB2-C715-4745-A8B2-14126EF533FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A64D7A2-53DB-40AE-A032-E61759EBA28B}"/>
+    <workbookView xWindow="23880" yWindow="-6750" windowWidth="24240" windowHeight="18240" activeTab="1" xr2:uid="{5A64D7A2-53DB-40AE-A032-E61759EBA28B}"/>
   </bookViews>
   <sheets>
     <sheet name="Street Estimates" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -1150,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CB2B78-1311-41BA-8B77-E57E89FD7212}">
   <dimension ref="B2:U47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1569,7 @@
         <v>23</v>
       </c>
       <c r="G15" s="31">
-        <v>1.6799999999999999E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
@@ -1602,7 +1604,7 @@
       </c>
       <c r="G20" s="31">
         <f>G12+G14*(G15-G12)</f>
-        <v>2.2679999999999999E-2</v>
+        <v>5.3536E-2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1633,7 +1635,7 @@
       </c>
       <c r="G23" s="31">
         <f>G22*G20+G21*G10*(1-G11)</f>
-        <v>2.7571492514565255E-2</v>
+        <v>3.2653603677573195E-2</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1719,23 +1721,23 @@
       </c>
       <c r="G32" s="35">
         <f>1/(1+$G$23)^K5</f>
-        <v>0.97316829756818668</v>
+        <v>0.9683789379504566</v>
       </c>
       <c r="H32" s="35">
         <f t="shared" ref="H32:K32" si="2">1/(1+$G$23)^L5</f>
-        <v>0.94705653539176271</v>
+        <v>0.93775776746605444</v>
       </c>
       <c r="I32" s="35">
         <f t="shared" si="2"/>
-        <v>0.92164539624802688</v>
+        <v>0.90810487091356917</v>
       </c>
       <c r="J32" s="35">
         <f t="shared" si="2"/>
-        <v>0.89691608122824906</v>
+        <v>0.87938963044291862</v>
       </c>
       <c r="K32" s="35">
         <f t="shared" si="2"/>
-        <v>0.87285029583042451</v>
+        <v>0.85158239637295807</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -1744,23 +1746,23 @@
       </c>
       <c r="G33" s="26">
         <f>K11*G32</f>
-        <v>13607.206994214866</v>
+        <v>13540.240357661829</v>
       </c>
       <c r="H33" s="26">
         <f t="shared" ref="H33:K33" si="3">L11*H32</f>
-        <v>13425.302611867548</v>
+        <v>13293.484955101661</v>
       </c>
       <c r="I33" s="26">
         <f t="shared" si="3"/>
-        <v>13260.827535298711</v>
+        <v>13066.003612856783</v>
       </c>
       <c r="J33" s="26">
         <f t="shared" si="3"/>
-        <v>12638.270454230296</v>
+        <v>12391.308637217904</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="3"/>
-        <v>11852.015475353988</v>
+        <v>11563.228870477662</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1773,7 +1775,7 @@
       <c r="F34" s="11"/>
       <c r="K34">
         <f>K32*G29</f>
-        <v>242791.16543789505</v>
+        <v>236875.30779270566</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1782,7 +1784,7 @@
       </c>
       <c r="F35" s="38">
         <f>SUM(G33:K34)</f>
-        <v>307574.78850886045</v>
+        <v>300729.57422602148</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1832,7 +1834,7 @@
       </c>
       <c r="F42" s="38">
         <f>F35+F38-F41-F40</f>
-        <v>277248.78850886045</v>
+        <v>270403.57422602148</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -1852,7 +1854,7 @@
       </c>
       <c r="F45" s="41">
         <f>F42/F44</f>
-        <v>518.99810653100042</v>
+        <v>506.1841524260978</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1861,7 +1863,7 @@
       </c>
       <c r="F46" s="41">
         <f>F45-248.48</f>
-        <v>270.5181065310004</v>
+        <v>257.70415242609783</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>